<commit_message>
v2 - 15mm dd-shaft and linear bearings
</commit_message>
<xml_diff>
--- a/calcs/Motor and Gear Sizing_v2.xlsx
+++ b/calcs/Motor and Gear Sizing_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\Ball Launcher\Version 2\sizing calculations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdalg\code\chuck_model\calcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CC9026-B231-4932-A34A-918A6A9CD7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09D2DBC-47B4-44CE-B2AE-8F6B31AF4FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4AEC8417-F2BC-4921-A4C3-11F562BCC427}"/>
+    <workbookView xWindow="38865" yWindow="3885" windowWidth="28800" windowHeight="15345" xr2:uid="{4AEC8417-F2BC-4921-A4C3-11F562BCC427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2030,7 +2030,7 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -2085,7 +2085,7 @@
         <v>36</v>
       </c>
       <c r="B10">
-        <v>12.5</v>
+        <v>12.6</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -2115,7 +2115,7 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -2126,7 +2126,7 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
         <v>24</v>
@@ -2137,7 +2137,7 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
@@ -2148,7 +2148,7 @@
         <v>26</v>
       </c>
       <c r="B17">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
@@ -2178,7 +2178,7 @@
         <v>30</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
         <v>19</v>
@@ -2193,7 +2193,7 @@
       </c>
       <c r="B22">
         <f>B20+B21</f>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
         <v>19</v>
@@ -2252,7 +2252,7 @@
       </c>
       <c r="B30">
         <f>B4*B6</f>
-        <v>672</v>
+        <v>640</v>
       </c>
       <c r="C30" t="str">
         <f>C4</f>
@@ -2268,7 +2268,7 @@
       </c>
       <c r="B31">
         <f>2*B30/(B22/10)</f>
-        <v>395.29411764705884</v>
+        <v>387.87878787878788</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
@@ -2283,7 +2283,7 @@
       </c>
       <c r="B32" s="6">
         <f>B31/9.81</f>
-        <v>40.295017089404567</v>
+        <v>39.539122107929444</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
@@ -2334,7 +2334,7 @@
       </c>
       <c r="B37">
         <f>PI()*B22</f>
-        <v>106.81415022205297</v>
+        <v>103.67255756846318</v>
       </c>
       <c r="C37" t="s">
         <v>19</v>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="B38" s="7">
         <f>(B16+0.5)/B15</f>
-        <v>0.59375</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="D38" t="s">
         <v>54</v>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="B39" s="6">
         <f>B37*B38</f>
-        <v>63.420901694343954</v>
+        <v>71.994831644766094</v>
       </c>
       <c r="C39" t="s">
         <v>19</v>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="B42">
         <f>B9/B10</f>
-        <v>1.2</v>
+        <v>1.1904761904761905</v>
       </c>
       <c r="D42" t="s">
         <v>73</v>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="B44">
         <f>B9*B10^2/(3+1.8*(B10/B9))</f>
-        <v>520.83333333333337</v>
+        <v>527.79255319148922</v>
       </c>
       <c r="C44" t="s">
         <v>66</v>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="B45" s="8">
         <f>(B43-B44)/B43</f>
-        <v>0.21404966374372666</v>
+        <v>0.20354802946353673</v>
       </c>
       <c r="D45" t="s">
         <v>63</v>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="B46">
         <f>(B30*10)/MIN(B43:B44)</f>
-        <v>12.902399999999998</v>
+        <v>12.12597631645251</v>
       </c>
       <c r="C46" t="s">
         <v>65</v>
@@ -2465,7 +2465,7 @@
       </c>
       <c r="B48" s="6">
         <f>B47/B46</f>
-        <v>1.5652126736111114</v>
+        <v>1.6654329080784571</v>
       </c>
       <c r="D48" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
add spring sizing, exit velocity, and launch range to calc
</commit_message>
<xml_diff>
--- a/calcs/Motor and Gear Sizing_v2.xlsx
+++ b/calcs/Motor and Gear Sizing_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdalg\code\chuck_model\calcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09D2DBC-47B4-44CE-B2AE-8F6B31AF4FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30EB4E8-7865-4758-AA5B-A95DD59AC1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38865" yWindow="3885" windowWidth="28800" windowHeight="15345" xr2:uid="{4AEC8417-F2BC-4921-A4C3-11F562BCC427}"/>
+    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15345" xr2:uid="{4AEC8417-F2BC-4921-A4C3-11F562BCC427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="168">
   <si>
     <t>Parameter</t>
   </si>
@@ -65,15 +65,9 @@
     <t>kgf</t>
   </si>
   <si>
-    <t>64:1 gear reduction</t>
-  </si>
-  <si>
     <t>Motor Sizing</t>
   </si>
   <si>
-    <t>Range Sizing</t>
-  </si>
-  <si>
     <t>Inputs</t>
   </si>
   <si>
@@ -152,15 +146,9 @@
     <t>Outputs</t>
   </si>
   <si>
-    <t>output force</t>
-  </si>
-  <si>
     <t>speed at wheel</t>
   </si>
   <si>
-    <t>torque at wheel</t>
-  </si>
-  <si>
     <t>launch period</t>
   </si>
   <si>
@@ -173,12 +161,6 @@
     <t>gear ratio including slip/wheel gears</t>
   </si>
   <si>
-    <t>theoretical max torque output at wheel</t>
-  </si>
-  <si>
-    <t>theoretical force output to rope</t>
-  </si>
-  <si>
     <t>wheel speed</t>
   </si>
   <si>
@@ -263,13 +245,310 @@
     <t>factor of safety</t>
   </si>
   <si>
-    <t>ratio of actual_stress/allowable_stress (value &gt; 1.5 desired to account for yield)</t>
+    <t>Springs</t>
+  </si>
+  <si>
+    <t>N/mm</t>
+  </si>
+  <si>
+    <t>spring rate</t>
+  </si>
+  <si>
+    <t>free length</t>
+  </si>
+  <si>
+    <t>compressed length</t>
+  </si>
+  <si>
+    <t>number of spindles</t>
+  </si>
+  <si>
+    <t>springs per spindle</t>
+  </si>
+  <si>
+    <t>Spring Sizing</t>
+  </si>
+  <si>
+    <t>Starting Position</t>
+  </si>
+  <si>
+    <t>pad resting position</t>
+  </si>
+  <si>
+    <t>distance from bottom of end cap to top of spindle pad</t>
+  </si>
+  <si>
+    <t>linear bearing height</t>
+  </si>
+  <si>
+    <t>distance from bottom of end cap to bottom of linear bearing</t>
+  </si>
+  <si>
+    <t>spindle spring free length</t>
+  </si>
+  <si>
+    <t>length after rope tensioning</t>
+  </si>
+  <si>
+    <t>length at max compression</t>
+  </si>
+  <si>
+    <t>spindle spring max compr.</t>
+  </si>
+  <si>
+    <t>max compression margin</t>
+  </si>
+  <si>
+    <t>uncompressed length of stacked springs on spindle</t>
+  </si>
+  <si>
+    <t>minimum possible spring compressed length</t>
+  </si>
+  <si>
+    <t>combined spring length after rope tensioning</t>
+  </si>
+  <si>
+    <t>minimum combined spring length during launch</t>
+  </si>
+  <si>
+    <t>difference between max compressed length during launch vs max possible spring compressed length (should be &gt; 0)</t>
+  </si>
+  <si>
+    <t>force at max compression total</t>
+  </si>
+  <si>
+    <t>uncompressed length of individual spring</t>
+  </si>
+  <si>
+    <t>fully compressed length of individual spring</t>
+  </si>
+  <si>
+    <t>number of spindles connected to ball pad</t>
+  </si>
+  <si>
+    <t>number of springs per spindle</t>
+  </si>
+  <si>
+    <t>Stroke Sizing</t>
+  </si>
+  <si>
+    <t>spring rate of selected springs (determined experimentally for single spring)</t>
+  </si>
+  <si>
+    <t>spring rate per spindle</t>
+  </si>
+  <si>
+    <t>spring rate total</t>
+  </si>
+  <si>
+    <t>effective spring rate per spindle (based on series spring equations)</t>
+  </si>
+  <si>
+    <t>effective spring rate total (based on parallel spring equations)</t>
+  </si>
+  <si>
+    <t>lbf</t>
+  </si>
+  <si>
+    <t>Alternate Units</t>
+  </si>
+  <si>
+    <t>launch angle</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>orientation of launch tube relative to horizontal</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>assumed mass of ball</t>
+  </si>
+  <si>
+    <t>initial force</t>
+  </si>
+  <si>
+    <t>final force</t>
+  </si>
+  <si>
+    <t>force exerted on ball at initiation of launch</t>
+  </si>
+  <si>
+    <t>force exerted on ball at end of launch (assumes all force transferred at end of stroke)</t>
+  </si>
+  <si>
+    <t>Masses</t>
+  </si>
+  <si>
+    <t>assumed mass of pad assembly</t>
+  </si>
+  <si>
+    <t>pad assembly</t>
+  </si>
+  <si>
+    <t>ball</t>
+  </si>
+  <si>
+    <t>total mass to accelerate</t>
+  </si>
+  <si>
+    <t>combined mass of ball and pad</t>
+  </si>
+  <si>
+    <t>average force</t>
+  </si>
+  <si>
+    <t>average acceleration</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>m/s^2</t>
+  </si>
+  <si>
+    <t>average acceleration over course of launch</t>
+  </si>
+  <si>
+    <t>Efficiencies</t>
+  </si>
+  <si>
+    <t>linear bearings</t>
+  </si>
+  <si>
+    <t>force lost to friction</t>
+  </si>
+  <si>
+    <t>average force lost to friction (arbitrarily assumed)</t>
+  </si>
+  <si>
+    <t>average theoretical force</t>
+  </si>
+  <si>
+    <t>theoretical average force exerted on ball over course of launch</t>
+  </si>
+  <si>
+    <t>average force exerted on ball over course of launch after friction</t>
+  </si>
+  <si>
+    <t>launch duration</t>
+  </si>
+  <si>
+    <t>distance travelled</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>duration of launch</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>exit velocity</t>
+  </si>
+  <si>
+    <t>theoretical exit velocity</t>
+  </si>
+  <si>
+    <t>Exit Velocity</t>
+  </si>
+  <si>
+    <t>Launch Range</t>
+  </si>
+  <si>
+    <t>time of flight</t>
+  </si>
+  <si>
+    <t>Horizontal velocity</t>
+  </si>
+  <si>
+    <t>Vertical velocity</t>
+  </si>
+  <si>
+    <t>horizontal component of velocity</t>
+  </si>
+  <si>
+    <t>vertical component of velocity</t>
+  </si>
+  <si>
+    <t>duration during which ball is in flight</t>
+  </si>
+  <si>
+    <t>distance travelled during launch (acceleration distance)</t>
+  </si>
+  <si>
+    <t>max height</t>
+  </si>
+  <si>
+    <t>max distance</t>
+  </si>
+  <si>
+    <t>horizontal distance travelled during flight (assumes initial height and air resistance are negligible for simplicity)</t>
+  </si>
+  <si>
+    <t>max height during flight (assumes initial height is negligible for simplicity)</t>
+  </si>
+  <si>
+    <t>16:1 gear reduction</t>
+  </si>
+  <si>
+    <t>efficiency of linear bearings at allowing spindles to move freely (approximated based on launch test results)</t>
+  </si>
+  <si>
+    <t>max force total</t>
+  </si>
+  <si>
+    <t>initial rope tension</t>
+  </si>
+  <si>
+    <t>force applied to rope due to initial tensioning process</t>
+  </si>
+  <si>
+    <t>gearbox efficiency (based on observation - very approximate)</t>
+  </si>
+  <si>
+    <t>gearbox</t>
+  </si>
+  <si>
+    <t>ratio of actual_stress/allowable_stress (target &gt; 1.5 if possible)</t>
+  </si>
+  <si>
+    <t>actual avail. torque at wheel</t>
+  </si>
+  <si>
+    <t>theoretical max torque output available from motor at wheel</t>
+  </si>
+  <si>
+    <t>actual torque output available at wheel after losses due to efficiency of gearbox</t>
+  </si>
+  <si>
+    <t>required torque</t>
+  </si>
+  <si>
+    <t>torque required at wheel</t>
+  </si>
+  <si>
+    <t>output torque margin</t>
+  </si>
+  <si>
+    <t>ideal avail. torque at wheel</t>
+  </si>
+  <si>
+    <t>margin of available output torque vs torque required to fully compress springs (target &gt; 1.2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -360,7 +639,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -369,7 +648,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -393,16 +675,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>537333</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>2549</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>51558</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>164474</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -417,7 +699,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11791950" y="647700"/>
+          <a:off x="12525375" y="428625"/>
           <a:ext cx="5290308" cy="2402849"/>
           <a:chOff x="12068175" y="571500"/>
           <a:chExt cx="5290308" cy="2402849"/>
@@ -1591,7 +1873,7 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3219450" cy="781240"/>
@@ -1659,6 +1941,79 @@
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
             <a:t>Extra margin should be designed in to protect against yielding. Target minimum FOS of 1.5.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3219450" cy="609013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="TextBox 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE4341FB-5CC0-484C-8276-5FD16DAEBA4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11125200" y="14897100"/>
+          <a:ext cx="3219450" cy="609013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>Exit velocity and launch range calculations are criminally approximate. Intended</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t> for rough sizing and relative comparison only.</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
@@ -1986,7 +2341,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287A575A-2F0B-464A-B6A3-1ED0F263129A}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:H99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1998,7 +2353,7 @@
     <col min="4" max="4" width="126.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2011,23 +2366,29 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
       </c>
       <c r="B4">
         <v>40</v>
@@ -2039,12 +2400,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5">
-        <v>320</v>
+        <v>480</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -2053,422 +2414,1016 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9">
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10">
         <v>12.6</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>21</v>
       </c>
       <c r="B14">
         <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B20">
         <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <f>B20+B21</f>
         <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="B25">
-        <v>35</v>
+        <f>(15/2.205*9.81)/(50-15)</f>
+        <v>1.9067055393586008</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26">
+        <v>50</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>10</v>
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32">
+        <v>128</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33">
+        <v>4.5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37">
+        <f>60+2.5*8</f>
+        <v>80</v>
+      </c>
+      <c r="C37" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38">
+        <v>60</v>
+      </c>
+      <c r="C38" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" s="7">
+        <v>0.22</v>
+      </c>
+      <c r="D41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>158</v>
+      </c>
+      <c r="B42" s="7">
+        <v>0.65</v>
+      </c>
+      <c r="D42" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45">
+        <v>35</v>
+      </c>
+      <c r="C45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>43</v>
       </c>
-      <c r="B29">
+      <c r="B49">
+        <f>PI()*B22</f>
+        <v>103.67255756846318</v>
+      </c>
+      <c r="C49" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="7">
+        <f>(B16+0.5)/B15</f>
+        <v>0.69444444444444442</v>
+      </c>
+      <c r="D50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" s="6">
+        <f>B49*B50</f>
+        <v>71.994831644766094</v>
+      </c>
+      <c r="C51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54">
+        <f>B29*B26</f>
+        <v>150</v>
+      </c>
+      <c r="C54" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55">
+        <f>B29*B27</f>
+        <v>45</v>
+      </c>
+      <c r="D55" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56">
+        <f>B32-B33</f>
+        <v>123.5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57">
+        <f>B56-B51</f>
+        <v>51.505168355233906</v>
+      </c>
+      <c r="C57" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" s="6">
+        <f>B57-B55</f>
+        <v>6.5051683552339057</v>
+      </c>
+      <c r="C58" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59">
+        <f>1/(B29*(1/B25))</f>
+        <v>0.63556851311953366</v>
+      </c>
+      <c r="C59" t="s">
+        <v>70</v>
+      </c>
+      <c r="D59" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>100</v>
+      </c>
+      <c r="B60">
+        <f>B59*B28</f>
+        <v>2.5422740524781346</v>
+      </c>
+      <c r="C60" t="s">
+        <v>70</v>
+      </c>
+      <c r="D60" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>155</v>
+      </c>
+      <c r="B61" s="6">
+        <f>(B54-B56)*B60</f>
+        <v>67.370262390670575</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" t="s">
+        <v>156</v>
+      </c>
+      <c r="E61" s="9">
+        <f>B61/9.81</f>
+        <v>6.8675089083252363</v>
+      </c>
+      <c r="F61" t="s">
+        <v>8</v>
+      </c>
+      <c r="G61" s="9">
+        <f>E61*2.205</f>
+        <v>15.142857142857146</v>
+      </c>
+      <c r="H61" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>154</v>
+      </c>
+      <c r="B62" s="6">
+        <f>(B54-B57)*B60</f>
+        <v>250.40085479369111</v>
+      </c>
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" t="s">
+        <v>92</v>
+      </c>
+      <c r="E62" s="9">
+        <f>B62/9.81</f>
+        <v>25.525061650733036</v>
+      </c>
+      <c r="F62" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="9">
+        <f>E62*2.205</f>
+        <v>56.28276093986635</v>
+      </c>
+      <c r="H62" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65">
         <f>B6*(B17/B14)</f>
         <v>16</v>
       </c>
-      <c r="D29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="D65" t="s">
         <v>40</v>
       </c>
-      <c r="B30">
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>166</v>
+      </c>
+      <c r="B66">
         <f>B4*B6</f>
         <v>640</v>
       </c>
-      <c r="C30" t="str">
+      <c r="C66" t="str">
         <f>C4</f>
         <v>N*cm</v>
       </c>
-      <c r="D30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31">
-        <f>2*B30/(B22/10)</f>
-        <v>387.87878787878788</v>
-      </c>
-      <c r="C31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="6">
-        <f>B31/9.81</f>
-        <v>39.539122107929444</v>
-      </c>
-      <c r="C32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33">
+      <c r="D66" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>160</v>
+      </c>
+      <c r="B67">
+        <f>B66*B42</f>
+        <v>416</v>
+      </c>
+      <c r="C67" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68">
+        <f>B62*(B22/10/2)</f>
+        <v>413.1614104095903</v>
+      </c>
+      <c r="C68" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>165</v>
+      </c>
+      <c r="B69" s="6">
+        <f>B67/B68</f>
+        <v>1.0068704131578883</v>
+      </c>
+      <c r="D69" t="s">
+        <v>167</v>
+      </c>
+      <c r="E69" s="11"/>
+      <c r="G69" s="11"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70">
         <f>B5/B6</f>
-        <v>20</v>
-      </c>
-      <c r="C33" t="str">
+        <v>30</v>
+      </c>
+      <c r="C70" t="str">
         <f>C5</f>
         <v>RPM</v>
       </c>
-      <c r="D33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="D70" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="6">
-        <f>60/B33</f>
-        <v>3</v>
-      </c>
-      <c r="C34" t="s">
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>37</v>
+      </c>
+      <c r="B71" s="6">
+        <f>60/B70</f>
+        <v>2</v>
+      </c>
+      <c r="C71" t="s">
+        <v>38</v>
+      </c>
+      <c r="D71" t="s">
         <v>42</v>
       </c>
-      <c r="D34" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B37">
-        <f>PI()*B22</f>
-        <v>103.67255756846318</v>
-      </c>
-      <c r="C37" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="7">
-        <f>(B16+0.5)/B15</f>
-        <v>0.69444444444444442</v>
-      </c>
-      <c r="D38" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39" s="6">
-        <f>B37*B38</f>
-        <v>71.994831644766094</v>
-      </c>
-      <c r="C39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42">
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74">
         <f>B9/B10</f>
         <v>1.1904761904761905</v>
       </c>
-      <c r="D42" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>60</v>
-      </c>
-      <c r="B43">
+      <c r="D74" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>54</v>
+      </c>
+      <c r="B75">
         <f>PI()*B9^3/16</f>
         <v>662.67970036659699</v>
       </c>
-      <c r="C43" t="s">
-        <v>66</v>
-      </c>
-      <c r="D43" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="C75" t="s">
+        <v>60</v>
+      </c>
+      <c r="D75" t="s">
         <v>61</v>
       </c>
-      <c r="B44">
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>55</v>
+      </c>
+      <c r="B76">
         <f>B9*B10^2/(3+1.8*(B10/B9))</f>
         <v>527.79255319148922</v>
       </c>
-      <c r="C44" t="s">
-        <v>66</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="C76" t="s">
+        <v>60</v>
+      </c>
+      <c r="D76" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>56</v>
+      </c>
+      <c r="B77" s="10">
+        <f>(B75-B76)/B75</f>
+        <v>0.20354802946353673</v>
+      </c>
+      <c r="D77" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>58</v>
+      </c>
+      <c r="B78" s="11">
+        <f>(B68*10)/MIN(B75:B76)</f>
+        <v>7.8281023085918866</v>
+      </c>
+      <c r="C78" t="s">
+        <v>59</v>
+      </c>
+      <c r="D78" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>64</v>
+      </c>
+      <c r="B79">
+        <f>0.577*B45</f>
+        <v>20.195</v>
+      </c>
+      <c r="C79" t="s">
+        <v>59</v>
+      </c>
+      <c r="D79" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>62</v>
-      </c>
-      <c r="B45" s="8">
-        <f>(B43-B44)/B43</f>
-        <v>0.20354802946353673</v>
-      </c>
-      <c r="D45" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46">
-        <f>(B30*10)/MIN(B43:B44)</f>
-        <v>12.12597631645251</v>
-      </c>
-      <c r="C46" t="s">
-        <v>65</v>
-      </c>
-      <c r="D46" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>70</v>
-      </c>
-      <c r="B47">
-        <f>0.577*B25</f>
-        <v>20.195</v>
-      </c>
-      <c r="C47" t="s">
-        <v>65</v>
-      </c>
-      <c r="D47" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>74</v>
-      </c>
-      <c r="B48" s="6">
-        <f>B47/B46</f>
-        <v>1.6654329080784571</v>
-      </c>
-      <c r="D48" t="s">
-        <v>75</v>
+      <c r="B80" s="6">
+        <f>B79/B78</f>
+        <v>2.5798078772979989</v>
+      </c>
+      <c r="D80" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>110</v>
+      </c>
+      <c r="B83">
+        <f>B62</f>
+        <v>250.40085479369111</v>
+      </c>
+      <c r="C83" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>111</v>
+      </c>
+      <c r="B84">
+        <f>B61</f>
+        <v>67.370262390670575</v>
+      </c>
+      <c r="C84" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>129</v>
+      </c>
+      <c r="B85">
+        <f>(B83+B84)/2</f>
+        <v>158.88555859218084</v>
+      </c>
+      <c r="C85" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>127</v>
+      </c>
+      <c r="B86">
+        <f>B85*(1-B41)</f>
+        <v>123.93073570190106</v>
+      </c>
+      <c r="C86" t="s">
+        <v>7</v>
+      </c>
+      <c r="D86" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>120</v>
+      </c>
+      <c r="B87">
+        <f>B85-B86</f>
+        <v>34.954822890279786</v>
+      </c>
+      <c r="C87" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>118</v>
+      </c>
+      <c r="B88">
+        <f>(B38+B37)/1000</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C88" t="s">
+        <v>122</v>
+      </c>
+      <c r="D88" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>121</v>
+      </c>
+      <c r="B89">
+        <f>B87/B88</f>
+        <v>249.67730635914131</v>
+      </c>
+      <c r="C89" t="s">
+        <v>123</v>
+      </c>
+      <c r="D89" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>133</v>
+      </c>
+      <c r="B90">
+        <f>B51/1000</f>
+        <v>7.1994831644766097E-2</v>
+      </c>
+      <c r="C90" t="s">
+        <v>134</v>
+      </c>
+      <c r="D90" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>132</v>
+      </c>
+      <c r="B91">
+        <f>SQRT(2*B90/B89)</f>
+        <v>2.4014642341321051E-2</v>
+      </c>
+      <c r="C91" t="s">
+        <v>38</v>
+      </c>
+      <c r="D91" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>137</v>
+      </c>
+      <c r="B92" s="9">
+        <f>B89*B91</f>
+        <v>5.9959112129592222</v>
+      </c>
+      <c r="C92" t="s">
+        <v>136</v>
+      </c>
+      <c r="D92" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>142</v>
+      </c>
+      <c r="B95">
+        <f>B92*COS(RADIANS(B34))</f>
+        <v>4.2397494780759235</v>
+      </c>
+      <c r="C95" t="s">
+        <v>136</v>
+      </c>
+      <c r="D95" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>143</v>
+      </c>
+      <c r="B96">
+        <f>B92*SIN(RADIANS(B34))</f>
+        <v>4.2397494780759235</v>
+      </c>
+      <c r="C96" t="s">
+        <v>136</v>
+      </c>
+      <c r="D96" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>141</v>
+      </c>
+      <c r="B97">
+        <f>2*B96/9.81</f>
+        <v>0.8643729822784757</v>
+      </c>
+      <c r="C97" t="s">
+        <v>38</v>
+      </c>
+      <c r="D97" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>148</v>
+      </c>
+      <c r="B98" s="9">
+        <f>B96^2/(2*9.81)</f>
+        <v>0.91618122511952416</v>
+      </c>
+      <c r="C98" t="s">
+        <v>134</v>
+      </c>
+      <c r="D98" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>149</v>
+      </c>
+      <c r="B99" s="9">
+        <f>B95*B97</f>
+        <v>3.6647249004780966</v>
+      </c>
+      <c r="C99" t="s">
+        <v>134</v>
+      </c>
+      <c r="D99" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2477,6 +3432,7 @@
     <hyperlink ref="D5" r:id="rId2" xr:uid="{7C706B24-42FE-446E-A507-CCBCC80B106D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v3 - redesign for larger gearbox, shafts, & springs
</commit_message>
<xml_diff>
--- a/calcs/Motor and Gear Sizing_v2.xlsx
+++ b/calcs/Motor and Gear Sizing_v2.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdalg\code\chuck_model\calcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30EB4E8-7865-4758-AA5B-A95DD59AC1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1694AAA-0A4E-4382-B9AA-1C886071FCCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15345" xr2:uid="{4AEC8417-F2BC-4921-A4C3-11F562BCC427}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4AEC8417-F2BC-4921-A4C3-11F562BCC427}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -494,9 +494,6 @@
     <t>max height during flight (assumes initial height is negligible for simplicity)</t>
   </si>
   <si>
-    <t>16:1 gear reduction</t>
-  </si>
-  <si>
     <t>efficiency of linear bearings at allowing spindles to move freely (approximated based on launch test results)</t>
   </si>
   <si>
@@ -540,6 +537,9 @@
   </si>
   <si>
     <t>margin of available output torque vs torque required to fully compress springs (target &gt; 1.2)</t>
+  </si>
+  <si>
+    <t>64:1 gear reduction</t>
   </si>
 </sst>
 </file>
@@ -590,7 +590,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -612,6 +612,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -639,7 +645,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -652,6 +658,7 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2391,7 +2398,7 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -2405,7 +2412,7 @@
         <v>14</v>
       </c>
       <c r="B5">
-        <v>480</v>
+        <v>600</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -2419,10 +2426,10 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2475,8 +2482,8 @@
       <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
-        <v>36</v>
+      <c r="B14" s="12">
+        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -2487,7 +2494,7 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
         <v>22</v>
@@ -2497,8 +2504,8 @@
       <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B16">
-        <v>12</v>
+      <c r="B16" s="12">
+        <v>16</v>
       </c>
       <c r="D16" t="s">
         <v>23</v>
@@ -2508,8 +2515,8 @@
       <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="B17">
-        <v>36</v>
+      <c r="B17" s="12">
+        <v>42</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -2524,8 +2531,8 @@
       <c r="A20" t="s">
         <v>26</v>
       </c>
-      <c r="B20">
-        <v>32</v>
+      <c r="B20" s="12">
+        <v>38</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -2539,7 +2546,7 @@
         <v>28</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -2554,7 +2561,7 @@
       </c>
       <c r="B22">
         <f>B20+B21</f>
-        <v>33</v>
+        <v>40.4</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -2573,8 +2580,8 @@
         <v>71</v>
       </c>
       <c r="B25">
-        <f>(15/2.205*9.81)/(50-15)</f>
-        <v>1.9067055393586008</v>
+        <f>(25/2.205*9.81)/(100-20)</f>
+        <v>1.3903061224489797</v>
       </c>
       <c r="C25" t="s">
         <v>70</v>
@@ -2588,7 +2595,7 @@
         <v>72</v>
       </c>
       <c r="B26">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
@@ -2602,7 +2609,7 @@
         <v>73</v>
       </c>
       <c r="B27">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
         <v>17</v>
@@ -2627,7 +2634,7 @@
         <v>75</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D29" t="s">
         <v>96</v>
@@ -2642,8 +2649,8 @@
       <c r="A32" t="s">
         <v>78</v>
       </c>
-      <c r="B32">
-        <v>128</v>
+      <c r="B32" s="12">
+        <v>145</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
@@ -2656,8 +2663,8 @@
       <c r="A33" t="s">
         <v>80</v>
       </c>
-      <c r="B33">
-        <v>4.5</v>
+      <c r="B33" s="12">
+        <v>3</v>
       </c>
       <c r="C33" t="s">
         <v>17</v>
@@ -2689,8 +2696,7 @@
       <c r="A37" t="s">
         <v>116</v>
       </c>
-      <c r="B37">
-        <f>60+2.5*8</f>
+      <c r="B37" s="12">
         <v>80</v>
       </c>
       <c r="C37" t="s">
@@ -2727,18 +2733,18 @@
         <v>0.22</v>
       </c>
       <c r="D41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B42" s="7">
         <v>0.65</v>
       </c>
       <c r="D42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2781,7 +2787,7 @@
       </c>
       <c r="B49">
         <f>PI()*B22</f>
-        <v>103.67255756846318</v>
+        <v>126.92034320502763</v>
       </c>
       <c r="C49" t="s">
         <v>17</v>
@@ -2796,7 +2802,7 @@
       </c>
       <c r="B50" s="7">
         <f>(B16+0.5)/B15</f>
-        <v>0.69444444444444442</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="D50" t="s">
         <v>48</v>
@@ -2808,7 +2814,7 @@
       </c>
       <c r="B51" s="6">
         <f>B49*B50</f>
-        <v>71.994831644766094</v>
+        <v>99.723126803950279</v>
       </c>
       <c r="C51" t="s">
         <v>17</v>
@@ -2828,7 +2834,7 @@
       </c>
       <c r="B54">
         <f>B29*B26</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="C54" t="s">
         <v>17</v>
@@ -2843,7 +2849,7 @@
       </c>
       <c r="B55">
         <f>B29*B27</f>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D55" t="s">
         <v>88</v>
@@ -2855,7 +2861,7 @@
       </c>
       <c r="B56">
         <f>B32-B33</f>
-        <v>123.5</v>
+        <v>142</v>
       </c>
       <c r="C56" t="s">
         <v>17</v>
@@ -2870,7 +2876,7 @@
       </c>
       <c r="B57">
         <f>B56-B51</f>
-        <v>51.505168355233906</v>
+        <v>42.276873196049721</v>
       </c>
       <c r="C57" t="s">
         <v>17</v>
@@ -2885,7 +2891,7 @@
       </c>
       <c r="B58" s="6">
         <f>B57-B55</f>
-        <v>6.5051683552339057</v>
+        <v>2.2768731960497206</v>
       </c>
       <c r="C58" t="s">
         <v>17</v>
@@ -2900,7 +2906,7 @@
       </c>
       <c r="B59">
         <f>1/(B29*(1/B25))</f>
-        <v>0.63556851311953366</v>
+        <v>0.69515306122448983</v>
       </c>
       <c r="C59" t="s">
         <v>70</v>
@@ -2915,7 +2921,7 @@
       </c>
       <c r="B60">
         <f>B59*B28</f>
-        <v>2.5422740524781346</v>
+        <v>2.7806122448979593</v>
       </c>
       <c r="C60" t="s">
         <v>70</v>
@@ -2926,28 +2932,28 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B61" s="6">
         <f>(B54-B56)*B60</f>
-        <v>67.370262390670575</v>
+        <v>161.27551020408163</v>
       </c>
       <c r="C61" t="s">
         <v>7</v>
       </c>
       <c r="D61" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E61" s="9">
         <f>B61/9.81</f>
-        <v>6.8675089083252363</v>
+        <v>16.439909297052154</v>
       </c>
       <c r="F61" t="s">
         <v>8</v>
       </c>
       <c r="G61" s="9">
         <f>E61*2.205</f>
-        <v>15.142857142857146</v>
+        <v>36.25</v>
       </c>
       <c r="H61" t="s">
         <v>103</v>
@@ -2955,11 +2961,11 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B62" s="6">
         <f>(B54-B57)*B60</f>
-        <v>250.40085479369111</v>
+        <v>438.56685769465764</v>
       </c>
       <c r="C62" t="s">
         <v>7</v>
@@ -2969,14 +2975,14 @@
       </c>
       <c r="E62" s="9">
         <f>B62/9.81</f>
-        <v>25.525061650733036</v>
+        <v>44.706101701799959</v>
       </c>
       <c r="F62" t="s">
         <v>8</v>
       </c>
       <c r="G62" s="9">
         <f>E62*2.205</f>
-        <v>56.28276093986635</v>
+        <v>98.576954252468909</v>
       </c>
       <c r="H62" t="s">
         <v>103</v>
@@ -2993,7 +2999,7 @@
       </c>
       <c r="B65">
         <f>B6*(B17/B14)</f>
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="D65" t="s">
         <v>40</v>
@@ -3001,60 +3007,60 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B66">
         <f>B4*B6</f>
-        <v>640</v>
+        <v>1600</v>
       </c>
       <c r="C66" t="str">
         <f>C4</f>
         <v>N*cm</v>
       </c>
       <c r="D66" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B67">
         <f>B66*B42</f>
-        <v>416</v>
+        <v>1040</v>
       </c>
       <c r="C67" t="s">
         <v>4</v>
       </c>
       <c r="D67" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B68">
         <f>B62*(B22/10/2)</f>
-        <v>413.1614104095903</v>
+        <v>885.9050525432084</v>
       </c>
       <c r="C68" t="s">
         <v>4</v>
       </c>
       <c r="D68" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B69" s="6">
         <f>B67/B68</f>
-        <v>1.0068704131578883</v>
+        <v>1.1739407028037872</v>
       </c>
       <c r="D69" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E69" s="11"/>
       <c r="G69" s="11"/>
@@ -3065,7 +3071,7 @@
       </c>
       <c r="B70">
         <f>B5/B6</f>
-        <v>30</v>
+        <v>9.375</v>
       </c>
       <c r="C70" t="str">
         <f>C5</f>
@@ -3081,7 +3087,7 @@
       </c>
       <c r="B71" s="6">
         <f>60/B70</f>
-        <v>2</v>
+        <v>6.4</v>
       </c>
       <c r="C71" t="s">
         <v>38</v>
@@ -3155,7 +3161,7 @@
       </c>
       <c r="B78" s="11">
         <f>(B68*10)/MIN(B75:B76)</f>
-        <v>7.8281023085918866</v>
+        <v>16.785099509007125</v>
       </c>
       <c r="C78" t="s">
         <v>59</v>
@@ -3185,10 +3191,10 @@
       </c>
       <c r="B80" s="6">
         <f>B79/B78</f>
-        <v>2.5798078772979989</v>
+        <v>1.203150448358264</v>
       </c>
       <c r="D80" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -3202,7 +3208,7 @@
       </c>
       <c r="B83">
         <f>B62</f>
-        <v>250.40085479369111</v>
+        <v>438.56685769465764</v>
       </c>
       <c r="C83" t="s">
         <v>7</v>
@@ -3217,7 +3223,7 @@
       </c>
       <c r="B84">
         <f>B61</f>
-        <v>67.370262390670575</v>
+        <v>161.27551020408163</v>
       </c>
       <c r="C84" t="s">
         <v>7</v>
@@ -3232,7 +3238,7 @@
       </c>
       <c r="B85">
         <f>(B83+B84)/2</f>
-        <v>158.88555859218084</v>
+        <v>299.92118394936961</v>
       </c>
       <c r="C85" t="s">
         <v>7</v>
@@ -3247,7 +3253,7 @@
       </c>
       <c r="B86">
         <f>B85*(1-B41)</f>
-        <v>123.93073570190106</v>
+        <v>233.93852348050831</v>
       </c>
       <c r="C86" t="s">
         <v>7</v>
@@ -3262,7 +3268,7 @@
       </c>
       <c r="B87">
         <f>B85-B86</f>
-        <v>34.954822890279786</v>
+        <v>65.982660468861297</v>
       </c>
       <c r="C87" t="s">
         <v>7</v>
@@ -3292,7 +3298,7 @@
       </c>
       <c r="B89">
         <f>B87/B88</f>
-        <v>249.67730635914131</v>
+        <v>471.30471763472349</v>
       </c>
       <c r="C89" t="s">
         <v>123</v>
@@ -3307,7 +3313,7 @@
       </c>
       <c r="B90">
         <f>B51/1000</f>
-        <v>7.1994831644766097E-2</v>
+        <v>9.9723126803950277E-2</v>
       </c>
       <c r="C90" t="s">
         <v>134</v>
@@ -3322,7 +3328,7 @@
       </c>
       <c r="B91">
         <f>SQRT(2*B90/B89)</f>
-        <v>2.4014642341321051E-2</v>
+        <v>2.0571314696408223E-2</v>
       </c>
       <c r="C91" t="s">
         <v>38</v>
@@ -3337,7 +3343,7 @@
       </c>
       <c r="B92" s="9">
         <f>B89*B91</f>
-        <v>5.9959112129592222</v>
+        <v>9.6953576643657158</v>
       </c>
       <c r="C92" t="s">
         <v>136</v>
@@ -3357,7 +3363,7 @@
       </c>
       <c r="B95">
         <f>B92*COS(RADIANS(B34))</f>
-        <v>4.2397494780759235</v>
+        <v>6.8556531505019649</v>
       </c>
       <c r="C95" t="s">
         <v>136</v>
@@ -3372,7 +3378,7 @@
       </c>
       <c r="B96">
         <f>B92*SIN(RADIANS(B34))</f>
-        <v>4.2397494780759235</v>
+        <v>6.855653150501964</v>
       </c>
       <c r="C96" t="s">
         <v>136</v>
@@ -3387,7 +3393,7 @@
       </c>
       <c r="B97">
         <f>2*B96/9.81</f>
-        <v>0.8643729822784757</v>
+        <v>1.3976866769626837</v>
       </c>
       <c r="C97" t="s">
         <v>38</v>
@@ -3402,7 +3408,7 @@
       </c>
       <c r="B98" s="9">
         <f>B96^2/(2*9.81)</f>
-        <v>0.91618122511952416</v>
+        <v>2.395513767583461</v>
       </c>
       <c r="C98" t="s">
         <v>134</v>
@@ -3417,7 +3423,7 @@
       </c>
       <c r="B99" s="9">
         <f>B95*B97</f>
-        <v>3.6647249004780966</v>
+        <v>9.5820550703338441</v>
       </c>
       <c r="C99" t="s">
         <v>134</v>

</xml_diff>